<commit_message>
2015-2017 movie gross list
</commit_message>
<xml_diff>
--- a/2015_movie.xlsx
+++ b/2015_movie.xlsx
@@ -19,20 +19,31 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Inconsolata"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -41,12 +52,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -147,6 +159,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43253.0)</f>
         <v>43253</v>
       </c>
+      <c r="J2" s="3" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("importxml(""https://www.boxofficemojo.com/yearly/chart/?view=releasedate&amp;view2=domestic&amp;yr=2015&amp;sort=gross&amp;order=DESC&amp;p=.htm"", ""//*[@id='body']/table[3]/tr/td[1]/table[1]/tr/td[2]/table[1]/tr/td/table[1]/tr/td/table[1]/tr/td[2]/b/a/@href"")"),"/movies/?id=starwars7.htm")</f>
+        <v>/movies/?id=starwars7.htm</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -185,6 +201,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43423.0)</f>
         <v>43423</v>
       </c>
+      <c r="J3" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=jurassicpark4.htm")</f>
+        <v>/movies/?id=jurassicpark4.htm</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -223,6 +243,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43381.0)</f>
         <v>43381</v>
       </c>
+      <c r="J4" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=avengers2.htm")</f>
+        <v>/movies/?id=avengers2.htm</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -261,6 +285,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43444.0)</f>
         <v>43444</v>
       </c>
+      <c r="J5" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pixar2014.htm")</f>
+        <v>/movies/?id=pixar2014.htm</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -299,6 +327,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43305.0)</f>
         <v>43305</v>
       </c>
+      <c r="J6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=fast7.htm")</f>
+        <v>/movies/?id=fast7.htm</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -337,6 +369,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43451.0)</f>
         <v>43451</v>
       </c>
+      <c r="J7" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=minions.htm")</f>
+        <v>/movies/?id=minions.htm</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -375,6 +411,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43156.0)</f>
         <v>43156</v>
       </c>
+      <c r="J8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=hungergames4.htm")</f>
+        <v>/movies/?id=hungergames4.htm</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -413,6 +453,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43176.0)</f>
         <v>43176</v>
       </c>
+      <c r="J9" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=scott2016.htm")</f>
+        <v>/movies/?id=scott2016.htm</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -451,6 +495,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43360.0)</f>
         <v>43360</v>
       </c>
+      <c r="J10" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=cinderella2015.htm")</f>
+        <v>/movies/?id=cinderella2015.htm</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -489,6 +537,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43197.0)</f>
         <v>43197</v>
       </c>
+      <c r="J11" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=bond24.htm")</f>
+        <v>/movies/?id=bond24.htm</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -527,6 +579,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43402.0)</f>
         <v>43402</v>
       </c>
+      <c r="J12" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=mi5.htm")</f>
+        <v>/movies/?id=mi5.htm</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -565,6 +621,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43311.0)</f>
         <v>43311</v>
       </c>
+      <c r="J13" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pitchperfect2.htm")</f>
+        <v>/movies/?id=pitchperfect2.htm</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -603,6 +663,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43246.0)</f>
         <v>43246</v>
       </c>
+      <c r="J14" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=revenant.htm")</f>
+        <v>/movies/?id=revenant.htm</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -641,6 +705,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43451.0)</f>
         <v>43451</v>
       </c>
+      <c r="J15" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=antman.htm")</f>
+        <v>/movies/?id=antman.htm</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -679,6 +747,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43353.0)</f>
         <v>43353</v>
       </c>
+      <c r="J16" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=happysmekday.htm")</f>
+        <v>/movies/?id=happysmekday.htm</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -717,6 +789,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43162.0)</f>
         <v>43162</v>
       </c>
+      <c r="J17" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=hoteltransylvania2.htm")</f>
+        <v>/movies/?id=hoteltransylvania2.htm</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -755,6 +831,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43227.0)</f>
         <v>43227</v>
       </c>
+      <c r="J18" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=fiftyshadesofgrey.htm")</f>
+        <v>/movies/?id=fiftyshadesofgrey.htm</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -793,6 +873,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43248.0)</f>
         <v>43248</v>
       </c>
+      <c r="J19" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=spongebob2.htm")</f>
+        <v>/movies/?id=spongebob2.htm</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -831,6 +915,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43395.0)</f>
         <v>43395</v>
       </c>
+      <c r="J20" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=straightouttacompton.htm")</f>
+        <v>/movies/?id=straightouttacompton.htm</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -869,6 +957,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43388.0)</f>
         <v>43388</v>
       </c>
+      <c r="J21" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=sanandreas.htm")</f>
+        <v>/movies/?id=sanandreas.htm</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -907,6 +999,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43367.0)</f>
         <v>43367</v>
       </c>
+      <c r="J22" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=furyroad.htm")</f>
+        <v>/movies/?id=furyroad.htm</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -945,6 +1041,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43197.0)</f>
         <v>43197</v>
       </c>
+      <c r="J23" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=daddyshome.htm")</f>
+        <v>/movies/?id=daddyshome.htm</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -983,6 +1083,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J24" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=insurgent.htm")</f>
+        <v>/movies/?id=insurgent.htm</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -1021,6 +1125,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43190.0)</f>
         <v>43190</v>
       </c>
+      <c r="J25" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=peanuts2015.htm")</f>
+        <v>/movies/?id=peanuts2015.htm</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -1059,6 +1167,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=secretservice.htm")</f>
+        <v>/movies/?id=secretservice.htm</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -1097,6 +1209,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43197.0)</f>
         <v>43197</v>
       </c>
+      <c r="J27" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pixar2013.htm")</f>
+        <v>/movies/?id=pixar2013.htm</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -1135,6 +1251,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43381.0)</f>
         <v>43381</v>
       </c>
+      <c r="J28" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=susancooper.htm")</f>
+        <v>/movies/?id=susancooper.htm</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -1173,6 +1293,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43388.0)</f>
         <v>43388</v>
       </c>
+      <c r="J29" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=trainwreck15.htm")</f>
+        <v>/movies/?id=trainwreck15.htm</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1211,6 +1335,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43162.0)</f>
         <v>43162</v>
       </c>
+      <c r="J30" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=creed.htm")</f>
+        <v>/movies/?id=creed.htm</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1249,6 +1377,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43360.0)</f>
         <v>43360</v>
       </c>
+      <c r="J31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=1952.htm")</f>
+        <v>/movies/?id=1952.htm</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -1287,6 +1419,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J32" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=gethard.htm")</f>
+        <v>/movies/?id=gethard.htm</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -1325,6 +1461,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43360.0)</f>
         <v>43360</v>
       </c>
+      <c r="J33" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=terminator2015.htm")</f>
+        <v>/movies/?id=terminator2015.htm</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1363,6 +1503,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43234.0)</f>
         <v>43234</v>
       </c>
+      <c r="J34" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=taken3.htm")</f>
+        <v>/movies/?id=taken3.htm</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -1401,6 +1545,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43169.0)</f>
         <v>43169</v>
       </c>
+      <c r="J35" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=nest.htm")</f>
+        <v>/movies/?id=nest.htm</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1439,6 +1587,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43239.0)</f>
         <v>43239</v>
       </c>
+      <c r="J36" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=alvin4.htm")</f>
+        <v>/movies/?id=alvin4.htm</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -1477,6 +1629,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43121.0)</f>
         <v>43121</v>
       </c>
+      <c r="J37" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=mazerunner2.htm")</f>
+        <v>/movies/?id=mazerunner2.htm</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -1515,6 +1671,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43339.0)</f>
         <v>43339</v>
       </c>
+      <c r="J38" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=ted2.htm")</f>
+        <v>/movies/?id=ted2.htm</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -1553,6 +1713,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43149.0)</f>
         <v>43149</v>
       </c>
+      <c r="J39" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=goosebumps.htm")</f>
+        <v>/movies/?id=goosebumps.htm</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -1591,6 +1755,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43412.0)</f>
         <v>43412</v>
       </c>
+      <c r="J40" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pixels.htm")</f>
+        <v>/movies/?id=pixels.htm</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -1629,6 +1797,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43269.0)</f>
         <v>43269</v>
       </c>
+      <c r="J41" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=paddington.htm")</f>
+        <v>/movies/?id=paddington.htm</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -1667,6 +1839,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43107.0)</f>
         <v>43107</v>
       </c>
+      <c r="J42" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=intern.htm")</f>
+        <v>/movies/?id=intern.htm</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1705,6 +1881,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43169.0)</f>
         <v>43169</v>
       </c>
+      <c r="J43" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=coldwar2015.htm")</f>
+        <v>/movies/?id=coldwar2015.htm</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -1743,6 +1923,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43314.0)</f>
         <v>43314</v>
       </c>
+      <c r="J44" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=paulblart2.htm")</f>
+        <v>/movies/?id=paulblart2.htm</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -1781,6 +1965,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43197.0)</f>
         <v>43197</v>
       </c>
+      <c r="J45" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=bigshort.htm")</f>
+        <v>/movies/?id=bigshort.htm</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -1819,6 +2007,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43447.0)</f>
         <v>43447</v>
       </c>
+      <c r="J46" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=warroom2015.htm")</f>
+        <v>/movies/?id=warroom2015.htm</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -1857,6 +2049,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43367.0)</f>
         <v>43367</v>
       </c>
+      <c r="J47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=magicmike2.htm")</f>
+        <v>/movies/?id=magicmike2.htm</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -1895,6 +2091,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43430.0)</f>
         <v>43430</v>
       </c>
+      <c r="J48" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=blumhouse2015.htm")</f>
+        <v>/movies/?id=blumhouse2015.htm</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -1933,6 +2133,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43195.0)</f>
         <v>43195</v>
       </c>
+      <c r="J49" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=kevinhart15.htm")</f>
+        <v>/movies/?id=kevinhart15.htm</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -1971,6 +2175,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43437.0)</f>
         <v>43437</v>
       </c>
+      <c r="J50" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=whiteybulger15.htm")</f>
+        <v>/movies/?id=whiteybulger15.htm</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -2009,6 +2217,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43402.0)</f>
         <v>43402</v>
       </c>
+      <c r="J51" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=newline15.htm")</f>
+        <v>/movies/?id=newline15.htm</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -2047,6 +2259,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43437.0)</f>
         <v>43437</v>
       </c>
+      <c r="J52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=perfectguy.htm")</f>
+        <v>/movies/?id=perfectguy.htm</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -2085,6 +2301,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43176.0)</f>
         <v>43176</v>
       </c>
+      <c r="J53" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=joy.htm")</f>
+        <v>/movies/?id=joy.htm</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -2123,6 +2343,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43395.0)</f>
         <v>43395</v>
       </c>
+      <c r="J54" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=fantasticfour15.htm")</f>
+        <v>/movies/?id=fantasticfour15.htm</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -2161,6 +2385,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43218.0)</f>
         <v>43218</v>
       </c>
+      <c r="J55" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=thehatefuleight.htm")</f>
+        <v>/movies/?id=thehatefuleight.htm</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -2199,6 +2427,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43227.0)</f>
         <v>43227</v>
       </c>
+      <c r="J56" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=focus2015.htm")</f>
+        <v>/movies/?id=focus2015.htm</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -2237,6 +2469,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43409.0)</f>
         <v>43409</v>
       </c>
+      <c r="J57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=southpaw2015.htm")</f>
+        <v>/movies/?id=southpaw2015.htm</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -2275,6 +2511,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43325.0)</f>
         <v>43325</v>
       </c>
+      <c r="J58" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=insidiouschapter3.htm")</f>
+        <v>/movies/?id=insidiouschapter3.htm</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -2313,6 +2553,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43318.0)</f>
         <v>43318</v>
       </c>
+      <c r="J59" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=poltergeist2015.htm")</f>
+        <v>/movies/?id=poltergeist2015.htm</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -2351,6 +2595,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43227.0)</f>
         <v>43227</v>
       </c>
+      <c r="J60" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=jupiterascending.htm")</f>
+        <v>/movies/?id=jupiterascending.htm</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -2389,6 +2637,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43114.0)</f>
         <v>43114</v>
       </c>
+      <c r="J61" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=sicario.htm")</f>
+        <v>/movies/?id=sicario.htm</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -2427,6 +2679,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43395.0)</f>
         <v>43395</v>
       </c>
+      <c r="J62" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=uncle.htm")</f>
+        <v>/movies/?id=uncle.htm</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -2465,6 +2721,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43225.0)</f>
         <v>43225</v>
       </c>
+      <c r="J63" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=spotlight.htm")</f>
+        <v>/movies/?id=spotlight.htm</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -2503,6 +2763,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J64" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=mcfarland.htm")</f>
+        <v>/movies/?id=mcfarland.htm</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -2541,6 +2805,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43382.0)</f>
         <v>43382</v>
       </c>
+      <c r="J65" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=blumhousejuly2015.htm")</f>
+        <v>/movies/?id=blumhousejuly2015.htm</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -2579,6 +2847,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43430.0)</f>
         <v>43430</v>
       </c>
+      <c r="J66" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=everest2015.htm")</f>
+        <v>/movies/?id=everest2015.htm</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -2617,6 +2889,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43114.0)</f>
         <v>43114</v>
       </c>
+      <c r="J67" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=xmas2015.htm")</f>
+        <v>/movies/?id=xmas2015.htm</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -2655,6 +2931,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43121.0)</f>
         <v>43121</v>
       </c>
+      <c r="J68" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=krampus.htm")</f>
+        <v>/movies/?id=krampus.htm</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -2693,6 +2973,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43388.0)</f>
         <v>43388</v>
       </c>
+      <c r="J69" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=max2015.htm")</f>
+        <v>/movies/?id=max2015.htm</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -2731,6 +3015,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J70" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=ageofadaline.htm")</f>
+        <v>/movies/?id=ageofadaline.htm</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -2769,6 +3057,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43246.0)</f>
         <v>43246</v>
       </c>
+      <c r="J71" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=brooklyn.htm")</f>
+        <v>/movies/?id=brooklyn.htm</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -2807,6 +3099,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43290.0)</f>
         <v>43290</v>
       </c>
+      <c r="J72" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=thelongestride.htm")</f>
+        <v>/movies/?id=thelongestride.htm</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -2845,6 +3141,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43171.0)</f>
         <v>43171</v>
       </c>
+      <c r="J73" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=boynextdoor.htm")</f>
+        <v>/movies/?id=boynextdoor.htm</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -2883,6 +3183,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43107.0)</f>
         <v>43107</v>
       </c>
+      <c r="J74" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pan.htm")</f>
+        <v>/movies/?id=pan.htm</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -2921,6 +3225,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43311.0)</f>
         <v>43311</v>
       </c>
+      <c r="J75" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=witherspoonvergara.htm")</f>
+        <v>/movies/?id=witherspoonvergara.htm</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -2959,6 +3267,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43176.0)</f>
         <v>43176</v>
       </c>
+      <c r="J76" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=concussion2015.htm")</f>
+        <v>/movies/?id=concussion2015.htm</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -2997,6 +3309,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43234.0)</f>
         <v>43234</v>
       </c>
+      <c r="J77" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=duff.htm")</f>
+        <v>/movies/?id=duff.htm</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -3035,6 +3351,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43325.0)</f>
         <v>43325</v>
       </c>
+      <c r="J78" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=womaningold.htm")</f>
+        <v>/movies/?id=womaningold.htm</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -3073,6 +3393,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43276.0)</f>
         <v>43276</v>
       </c>
+      <c r="J79" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=bestexotic2.htm")</f>
+        <v>/movies/?id=bestexotic2.htm</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -3111,6 +3435,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43248.0)</f>
         <v>43248</v>
       </c>
+      <c r="J80" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=cybernatural.htm")</f>
+        <v>/movies/?id=cybernatural.htm</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -3149,6 +3477,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43325.0)</f>
         <v>43325</v>
       </c>
+      <c r="J81" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=entourage.htm")</f>
+        <v>/movies/?id=entourage.htm</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -3187,6 +3519,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43388.0)</f>
         <v>43388</v>
       </c>
+      <c r="J82" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=papertowns.htm")</f>
+        <v>/movies/?id=papertowns.htm</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -3225,6 +3561,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43223.0)</f>
         <v>43223</v>
       </c>
+      <c r="J83" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=chappie.htm")</f>
+        <v>/movies/?id=chappie.htm</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -3263,6 +3603,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43430.0)</f>
         <v>43430</v>
       </c>
+      <c r="J84" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=crimsonpeak.htm")</f>
+        <v>/movies/?id=crimsonpeak.htm</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -3301,6 +3645,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43454.0)</f>
         <v>43454</v>
       </c>
+      <c r="J85" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=walkinthewoods.htm")</f>
+        <v>/movies/?id=walkinthewoods.htm</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -3339,6 +3687,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43156.0)</f>
         <v>43156</v>
       </c>
+      <c r="J86" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=pointbreak2015.htm")</f>
+        <v>/movies/?id=pointbreak2015.htm</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -3377,6 +3729,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43402.0)</f>
         <v>43402</v>
       </c>
+      <c r="J87" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=sinister2.htm")</f>
+        <v>/movies/?id=sinister2.htm</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -3415,6 +3771,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43465.0)</f>
         <v>43465</v>
       </c>
+      <c r="J88" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=lastwitchhunter.htm")</f>
+        <v>/movies/?id=lastwitchhunter.htm</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -3453,6 +3813,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43430.0)</f>
         <v>43430</v>
       </c>
+      <c r="J89" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=coup.htm")</f>
+        <v>/movies/?id=coup.htm</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -3491,6 +3855,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43384.0)</f>
         <v>43384</v>
       </c>
+      <c r="J90" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=rickiandtheflash.htm")</f>
+        <v>/movies/?id=rickiandtheflash.htm</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -3529,6 +3897,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43178.0)</f>
         <v>43178</v>
       </c>
+      <c r="J91" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=womaninblack2.htm")</f>
+        <v>/movies/?id=womaninblack2.htm</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -3567,6 +3939,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43227.0)</f>
         <v>43227</v>
       </c>
+      <c r="J92" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=runallnight.htm")</f>
+        <v>/movies/?id=runallnight.htm</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -3605,6 +3981,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43114.0)</f>
         <v>43114</v>
       </c>
+      <c r="J93" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=lovethecoopers.htm")</f>
+        <v>/movies/?id=lovethecoopers.htm</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -3643,6 +4023,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43262.0)</f>
         <v>43262</v>
       </c>
+      <c r="J94" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=lazarus.htm")</f>
+        <v>/movies/?id=lazarus.htm</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -3681,6 +4065,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43346.0)</f>
         <v>43346</v>
       </c>
+      <c r="J95" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=exmachina.htm")</f>
+        <v>/movies/?id=exmachina.htm</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -3719,6 +4107,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43142.0)</f>
         <v>43142</v>
       </c>
+      <c r="J96" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=heartofthesea.htm")</f>
+        <v>/movies/?id=heartofthesea.htm</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -3757,6 +4149,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43360.0)</f>
         <v>43360</v>
       </c>
+      <c r="J97" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=newlinehorror2015.htm")</f>
+        <v>/movies/?id=newlinehorror2015.htm</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -3795,6 +4191,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43388.0)</f>
         <v>43388</v>
       </c>
+      <c r="J98" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=hitman47.htm")</f>
+        <v>/movies/?id=hitman47.htm</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -3833,6 +4233,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43185.0)</f>
         <v>43185</v>
       </c>
+      <c r="J99" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=almanac.htm")</f>
+        <v>/movies/?id=almanac.htm</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -3871,6 +4275,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43234.0)</f>
         <v>43234</v>
       </c>
+      <c r="J100" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=blackorwhite.htm")</f>
+        <v>/movies/?id=blackorwhite.htm</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -3909,6 +4317,10 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43311.0)</f>
         <v>43311</v>
       </c>
+      <c r="J101" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"/movies/?id=crowe2014.htm")</f>
+        <v>/movies/?id=crowe2014.htm</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">

</xml_diff>